<commit_message>
Rename new file type and increase test coverage
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/accessioning_template_simple.xlsx
+++ b/docs/public/help/help_linked_docs/accessioning_template_simple.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/Documents/help_linked_docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{913F1F27-01B3-B54A-88C1-3A83FA4CD86A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D3809F3-5D73-6146-9EF9-F02E1AC617C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Age:</t>
   </si>
@@ -68,6 +68,12 @@
   </si>
   <si>
     <t>Unique Analysis ID*:</t>
+  </si>
+  <si>
+    <t>Case Files:</t>
+  </si>
+  <si>
+    <t>Genome Build:</t>
   </si>
 </sst>
 </file>
@@ -909,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,9 +937,12 @@
     <col min="13" max="13" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23.5" style="1" customWidth="1"/>
     <col min="15" max="15" width="15.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="21.83203125" customWidth="1"/>
+    <col min="17" max="17" width="24.33203125" customWidth="1"/>
+    <col min="18" max="18" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -981,6 +990,12 @@
       </c>
       <c r="P1" t="s">
         <v>6</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update simple accessioning forms
</commit_message>
<xml_diff>
--- a/docs/public/help/help_linked_docs/accessioning_template_simple.xlsx
+++ b/docs/public/help/help_linked_docs/accessioning_template_simple.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/drioux/CGAP/cgap-portal-2/docs/public/help/help_linked_docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5FE2CEC-40C1-1448-AA5A-EAE3FEB15D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCBA65A2-C28E-9B40-BCD8-1C6F633F3F6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Age:</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>Variant Type:</t>
+  </si>
+  <si>
+    <t>Tags:</t>
   </si>
 </sst>
 </file>
@@ -923,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -944,15 +947,15 @@
     <col min="12" max="12" width="16.6640625" customWidth="1"/>
     <col min="13" max="13" width="15.83203125" customWidth="1"/>
     <col min="14" max="14" width="23.5" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="21.83203125" customWidth="1"/>
-    <col min="17" max="17" width="24.33203125" customWidth="1"/>
-    <col min="18" max="18" width="14" customWidth="1"/>
-    <col min="19" max="19" width="12.83203125" customWidth="1"/>
-    <col min="20" max="20" width="15.1640625" customWidth="1"/>
+    <col min="15" max="16" width="15.83203125" style="1" customWidth="1"/>
+    <col min="17" max="17" width="21.83203125" customWidth="1"/>
+    <col min="18" max="18" width="24.33203125" customWidth="1"/>
+    <col min="19" max="19" width="14" customWidth="1"/>
+    <col min="20" max="20" width="12.83203125" customWidth="1"/>
+    <col min="21" max="21" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -998,19 +1001,22 @@
       <c r="O1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>